<commit_message>
update .xlsx file and run `python certs.py`
</commit_message>
<xml_diff>
--- a/fb.xlsx
+++ b/fb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Dev/github/PEDUtaunggalay/Certificate-Generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142ABB97-4F95-FD40-BF5A-578E89ACB81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B69609C-87D1-8E47-957E-ED884CC72306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="22280" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="500" windowWidth="24720" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,20 +33,28 @@
     <t>Name</t>
   </si>
   <si>
-    <t>sirai.waqar.ali@gmail.com</t>
+    <t>Saw Myint Win</t>
   </si>
   <si>
-    <t>Saw Thinkar Nay Htoo</t>
+    <t>sawmyintwin@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -69,14 +77,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -410,7 +421,7 @@
   <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="184" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -428,11 +439,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
+      <c r="A2" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -612,10 +623,13 @@
       <c r="B46" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{ADC3398F-2E79-4548-A5A7-20E2A0019F87}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding father's name text works
</commit_message>
<xml_diff>
--- a/fb.xlsx
+++ b/fb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Dev/github/PEDUtaunggalay/Certificate-Generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B69609C-87D1-8E47-957E-ED884CC72306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEC9350-57D1-704B-A928-74A91ED5396A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="500" windowWidth="24720" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Email</t>
   </si>
@@ -33,10 +33,22 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Saw Myint Win</t>
+    <t>sawmyintwin@gmail.com</t>
   </si>
   <si>
-    <t>sawmyintwin@gmail.com</t>
+    <t>Naw Nandar Oo</t>
+  </si>
+  <si>
+    <t>U Ba Htoo</t>
+  </si>
+  <si>
+    <t>Father</t>
+  </si>
+  <si>
+    <t>U Ba Aye</t>
+  </si>
+  <si>
+    <t>Nan Aye</t>
   </si>
 </sst>
 </file>
@@ -90,7 +102,10 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -111,11 +126,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B46" totalsRowShown="0">
-  <autoFilter ref="A1:B46" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="2">
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Email" dataDxfId="1"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Name" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C46" totalsRowShown="0">
+  <autoFilter ref="A1:C46" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="3">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Email" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Name" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{124D6FE6-91A4-E64E-AF99-062E8186A4F1}" name="Father" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -418,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="184" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -430,206 +446,263 @@
     <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{ADC3398F-2E79-4548-A5A7-20E2A0019F87}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{CDDECD1F-9D1B-FF49-B757-CBC83ABD00B2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
generate father's name and overlay photo
</commit_message>
<xml_diff>
--- a/fb.xlsx
+++ b/fb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Dev/github/PEDUtaunggalay/Certificate-Generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEC9350-57D1-704B-A928-74A91ED5396A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A362B27-ED74-4B4F-8C45-E4CBADB7804A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="500" windowWidth="24720" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Email</t>
   </si>
@@ -49,6 +49,18 @@
   </si>
   <si>
     <t>Nan Aye</t>
+  </si>
+  <si>
+    <t>Phlon No.</t>
+  </si>
+  <si>
+    <t>Photo</t>
+  </si>
+  <si>
+    <t>https://help.twitter.com/content/dam/help-twitter/brand/logo.png</t>
+  </si>
+  <si>
+    <t>https://www.seekpng.com/png/detail/280-2802791_moran-facebook-link-facebook-logo-black.png</t>
   </si>
 </sst>
 </file>
@@ -102,7 +114,10 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -126,12 +141,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C46" totalsRowShown="0">
-  <autoFilter ref="A1:C46" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="3">
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Email" dataDxfId="2"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Name" dataDxfId="1"/>
-    <tableColumn id="1" xr3:uid="{124D6FE6-91A4-E64E-AF99-062E8186A4F1}" name="Father" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B1:E46" totalsRowShown="0">
+  <autoFilter ref="B1:E46" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="4">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Email" dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Name" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{124D6FE6-91A4-E64E-AF99-062E8186A4F1}" name="Father" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{BE00FB85-2EFC-8D4B-9BB4-8D9DCA425405}" name="Photo" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -434,275 +450,339 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="184" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="184" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" customWidth="1"/>
+    <col min="2" max="2" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{ADC3398F-2E79-4548-A5A7-20E2A0019F87}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{CDDECD1F-9D1B-FF49-B757-CBC83ABD00B2}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{ADC3398F-2E79-4548-A5A7-20E2A0019F87}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{CDDECD1F-9D1B-FF49-B757-CBC83ABD00B2}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{D576EC2A-13C6-3049-BF15-40F737F07143}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{7D8E797D-B0F1-7D42-8F1E-0E2FC7955FA6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update codes for gender, father's name
</commit_message>
<xml_diff>
--- a/fb.xlsx
+++ b/fb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Dev/github/PEDUtaunggalay/Certificate-Generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A362B27-ED74-4B4F-8C45-E4CBADB7804A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB5572E-AAE3-2D44-8124-F2C510C877B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="500" windowWidth="24720" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,9 +36,6 @@
     <t>sawmyintwin@gmail.com</t>
   </si>
   <si>
-    <t>Naw Nandar Oo</t>
-  </si>
-  <si>
     <t>U Ba Htoo</t>
   </si>
   <si>
@@ -54,20 +51,23 @@
     <t>Phlon No.</t>
   </si>
   <si>
-    <t>Photo</t>
-  </si>
-  <si>
-    <t>https://help.twitter.com/content/dam/help-twitter/brand/logo.png</t>
-  </si>
-  <si>
-    <t>https://www.seekpng.com/png/detail/280-2802791_moran-facebook-link-facebook-logo-black.png</t>
+    <t>Nan Dae Thayi Sandar Aye</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +79,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -105,10 +113,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -147,7 +156,7 @@
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Email" dataDxfId="3"/>
     <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Name" dataDxfId="2"/>
     <tableColumn id="1" xr3:uid="{124D6FE6-91A4-E64E-AF99-062E8186A4F1}" name="Father" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{BE00FB85-2EFC-8D4B-9BB4-8D9DCA425405}" name="Photo" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{BE00FB85-2EFC-8D4B-9BB4-8D9DCA425405}" name="Gender" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -452,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="184" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="184" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -465,7 +474,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -474,7 +483,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
         <v>9</v>
@@ -488,12 +497,12 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -505,12 +514,12 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -776,13 +785,11 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{ADC3398F-2E79-4548-A5A7-20E2A0019F87}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{CDDECD1F-9D1B-FF49-B757-CBC83ABD00B2}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{D576EC2A-13C6-3049-BF15-40F737F07143}"/>
-    <hyperlink ref="E3" r:id="rId4" xr:uid="{7D8E797D-B0F1-7D42-8F1E-0E2FC7955FA6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>